<commit_message>
Changed Table names (invert S3 and S4)
</commit_message>
<xml_diff>
--- a/data/Table_S1_Sylvatic_DENV-2_Cynomolgus_Macaques.xlsx
+++ b/data/Table_S1_Sylvatic_DENV-2_Cynomolgus_Macaques.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trade-Off_Project_Cyno_Inf_Sylv" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Column Information" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -1367,7 +1367,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1385,10 +1385,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1420,15 +1416,15 @@
   </sheetPr>
   <dimension ref="A1:DB209"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="T5" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="1" topLeftCell="T50" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="T1" activeCellId="0" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
       <selection pane="bottomRight" activeCell="U23" activeCellId="0" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.48046875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.86"/>
@@ -1504,12 +1500,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="1" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="1" width="7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="92" min="88" style="1" width="11.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="92" min="88" style="1" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="1" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="11.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="1" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="1" width="11.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="97" style="1" width="11.47"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="97" style="1" width="11.46"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="53.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -31284,868 +31280,868 @@
   </sheetPr>
   <dimension ref="A1:B109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I103" activeCellId="0" sqref="I103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="5" width="11.77"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="1" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="1" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="1" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="1" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="1" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="1" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="1" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="1" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="1" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="1" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="1" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="1" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="1" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="1" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="1" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="1" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="1" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="1" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="1" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="6" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="6" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="6" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="6" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="6" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="6" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B60" s="6" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" s="6" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="6" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="1" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="1" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="1" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="1" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="1" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="1" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="1" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+      <c r="A70" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="s">
+      <c r="A71" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="1" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
+      <c r="A72" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="1" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="1" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="1" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
+      <c r="A75" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="1" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="s">
+      <c r="A76" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="s">
+      <c r="A77" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="1" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
+      <c r="A78" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="1" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="s">
+      <c r="A79" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="1" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="s">
+      <c r="A80" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="1" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="1" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
+      <c r="A82" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="1" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="s">
+      <c r="A83" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="1" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="1" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
+      <c r="A85" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="1" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="s">
+      <c r="A86" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="1" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="s">
+      <c r="A87" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
+      <c r="A88" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="1" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="5" t="s">
+      <c r="A89" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="1" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5" t="s">
+      <c r="A90" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="1" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="5" t="s">
+      <c r="A91" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="1" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="1" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="1" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="1" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="1" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5" t="s">
+      <c r="A96" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="1" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5" t="s">
+      <c r="A97" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="1" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5" t="s">
+      <c r="A98" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="1" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="s">
+      <c r="A99" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="1" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5" t="s">
+      <c r="A100" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="1" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5" t="s">
+      <c r="A101" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="1" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5" t="s">
+      <c r="A102" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="1" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="1" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
+      <c r="A104" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="1" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5" t="s">
+      <c r="A105" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="1" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5" t="s">
+      <c r="A106" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="1" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="1" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5" t="s">
+      <c r="A108" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="1" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="s">
+      <c r="A109" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="1" t="s">
         <v>384</v>
       </c>
     </row>

</xml_diff>